<commit_message>
Se actualizo el archivo de casos de pruebas
</commit_message>
<xml_diff>
--- a/Plan de casos de pruebas Página inmobiliaria.xlsx
+++ b/Plan de casos de pruebas Página inmobiliaria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juan.moncaleano\Desktop\testSeniorQA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD28C488-62E8-404E-BABE-E67B328170A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0509EFFB-F160-480A-9ABF-3BA855B7D368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{971977C5-60B5-46C4-9B8A-13F50930D89B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="81">
   <si>
     <t>No</t>
   </si>
@@ -256,6 +256,69 @@
 3. Debe elegir la fecha que desea programar la presentación (12 de Septiembre de 2022).
 4. Debe elegir y seleccionar una fecha para la presentación (1PM/3PM).
 5. Debe seleccionar la opción “Llamada en Zoom” en el switch.  6. Debe diligenciar el campo correo “juanmonca1075mail.com”   7. Debemos hacer clic en el botón que dice “Agendar Presentación”  8. Debemos esperar que pase a la siguiente ventana para poder diligenciar el campo Nombre Completo (“Juan Diego Moncaleano Quiñones”) 9. Debemos diligenciar el campo de Número de Teléfono  10. Hacemos clic en el botón “Agendar Presentación”  11. Esperamos que nos muestre el mensaje de confirmación de la presentación, y damos clic en el botón “Entrar al sitio”.</t>
+  </si>
+  <si>
+    <t>Nos debe mostrar una ventana modal donde seleccionamos la fecha y hora deseada para la presentación y el tipo de comucniación para la misma.</t>
+  </si>
+  <si>
+    <t>Nos debe mostrar una ventana modal donde seleccionamos la fecha y hora deseada para la presentación.</t>
+  </si>
+  <si>
+    <t>Nos debe mostrar una ventana modal donde seleccionamos la fecha deseada para la presentación.</t>
+  </si>
+  <si>
+    <t>Nos debe mostrar una ventana modal donde seleccionamos la fecha y hora deseada para la presentación y el tipo de comunicación para la misma.</t>
+  </si>
+  <si>
+    <t>Nos debe mostrar una ventana modal donde seleccionamos la fecha y hora deseada para la presentación y el tipo de comunicación para la misma y el campo de correo diligenciado.</t>
+  </si>
+  <si>
+    <t>Mostrará que la pagina se moverá hacia la parte inferior de la misma.</t>
+  </si>
+  <si>
+    <t>La página se desplazó hacia la parte inferior de la misma.</t>
+  </si>
+  <si>
+    <t>Se desplazó hacia la parte de debajo de la página y al dar clic sobre el boton "Presentación del proyecto" nos mostró la opción de selccionar la fecha y la fecha que elegimos.</t>
+  </si>
+  <si>
+    <t>Se desplazó hacia la parte de debajo de la página y al dar clic sobre el boton "Presentación del proyecto" nos mostró la opción de selccionar la fecha y la fecha que elegimos y la hora que se eligió.</t>
+  </si>
+  <si>
+    <t>Se desplazó hacia la parte de debajo de la página y al dar clic sobre el boton "Presentación del proyecto" nos mostró la opción de selccionar la fecha, la fecha que elegimos,  la hora y el tipo de comunicación.</t>
+  </si>
+  <si>
+    <t>Se desplazó hacia la parte de debajo de la página y al dar clic sobre el boton "Presentación del proyecto" nos mostró la opción de selccionar la fecha, la fecha que elegimos,  la hora, el tipo de comunicación y el correo del contacto que digitamos.</t>
+  </si>
+  <si>
+    <t>Nos debe mostrar una ventana modal donde seleccionamos la fecha y hora deseada para la presentación y el tipo de comunicación para la misma y el campo de correo diligenciado, luego daremos clic enel boton "Agendar Presentación" para que nos muestre el siguiente formulario.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nos muestra el siguiente formulario con los campos "Nombre completo" y "Número de teléfono". </t>
+  </si>
+  <si>
+    <t>Nos debe mostrar el campo de "Nombre completo" diligenciado.</t>
+  </si>
+  <si>
+    <t>Nos debe mostrar los campos "Nombre completo" y "Número de teléfono" diligenciados.</t>
+  </si>
+  <si>
+    <t>Nos muestra el campo "Nombre completo" diligenciado con la información que le hemos ingresado.</t>
+  </si>
+  <si>
+    <t>Nos muestra los campos "Nombre completo" y "Número de teléfono" diligenciados con la información que le hemos ingresado.</t>
+  </si>
+  <si>
+    <t>Nos debe mostar la ultima ventan con la información de la presentación programada, donde nos mostrará la fecha y hora que hemos elegido.</t>
+  </si>
+  <si>
+    <t>Al dar clic en el boton "Entrar al sitio" nos cierra la ventana modal y nos llevará de nuevo a la parte inferior de la página, luego nos envia a la parte superiod de la misma y por ultimo debe cerrar el navegador.</t>
+  </si>
+  <si>
+    <t>Nos muestrs una nueva ventana con la información pertinente a la reunión agendada.</t>
+  </si>
+  <si>
+    <t>Se cierra la ventana modal y nos redirige a la parte superior de lapágina, y por ultimo se cierró el navegador.</t>
   </si>
 </sst>
 </file>
@@ -675,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5F0F5A-9D07-45BB-9C4C-6759B21E0D3F}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,8 +805,12 @@
       <c r="F2" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="I2" s="4" t="s">
         <v>12</v>
       </c>
@@ -752,7 +819,7 @@
       </c>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -771,8 +838,12 @@
       <c r="F3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="4"/>
+      <c r="G3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="I3" s="4" t="s">
         <v>12</v>
       </c>
@@ -781,7 +852,7 @@
       </c>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -800,8 +871,12 @@
       <c r="F4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="G4" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="I4" s="4" t="s">
         <v>12</v>
       </c>
@@ -810,7 +885,7 @@
       </c>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -829,8 +904,12 @@
       <c r="F5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="G5" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="I5" s="4" t="s">
         <v>12</v>
       </c>
@@ -839,7 +918,7 @@
       </c>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -858,8 +937,12 @@
       <c r="F6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="G6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="I6" s="4" t="s">
         <v>12</v>
       </c>
@@ -868,7 +951,7 @@
       </c>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" ht="225" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -887,8 +970,12 @@
       <c r="F7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="G7" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="I7" s="4" t="s">
         <v>12</v>
       </c>
@@ -897,7 +984,7 @@
       </c>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="210" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -916,8 +1003,12 @@
       <c r="F8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="G8" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="I8" s="4" t="s">
         <v>12</v>
       </c>
@@ -926,7 +1017,7 @@
       </c>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" ht="255" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -945,8 +1036,12 @@
       <c r="F9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="G9" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="I9" s="4" t="s">
         <v>12</v>
       </c>
@@ -955,7 +1050,7 @@
       </c>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" ht="300" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="225" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -974,8 +1069,12 @@
       <c r="F10" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="G10" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="I10" s="4" t="s">
         <v>12</v>
       </c>
@@ -984,7 +1083,7 @@
       </c>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" ht="375" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="300" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1003,8 +1102,12 @@
       <c r="F11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="G11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="I11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1013,7 +1116,7 @@
       </c>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" ht="405" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="315" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1032,8 +1135,12 @@
       <c r="F12" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="G12" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="I12" s="4" t="s">
         <v>12</v>
       </c>
@@ -1061,8 +1168,12 @@
       <c r="F13" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="I13" s="7" t="s">
         <v>12</v>
       </c>
@@ -1090,8 +1201,12 @@
       <c r="F14" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="I14" s="4" t="s">
         <v>12</v>
       </c>

</xml_diff>